<commit_message>
Adicionado curva Roc-AUC para todas as classificacoes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -23691,7 +23691,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -23707,7 +23707,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -24131,7 +24131,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -24147,7 +24147,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -24379,7 +24379,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -24403,7 +24403,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -24419,7 +24419,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -24459,7 +24459,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -24531,7 +24531,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -24563,7 +24563,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -24643,7 +24643,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -25371,7 +25371,7 @@
         <v>212</v>
       </c>
       <c r="B212">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -25435,7 +25435,7 @@
         <v>220</v>
       </c>
       <c r="B220">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -25451,7 +25451,7 @@
         <v>222</v>
       </c>
       <c r="B222">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -25907,7 +25907,7 @@
         <v>279</v>
       </c>
       <c r="B279">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -25987,7 +25987,7 @@
         <v>289</v>
       </c>
       <c r="B289">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -26091,7 +26091,7 @@
         <v>302</v>
       </c>
       <c r="B302">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -26123,7 +26123,7 @@
         <v>306</v>
       </c>
       <c r="B306">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -26219,7 +26219,7 @@
         <v>318</v>
       </c>
       <c r="B318">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -26283,7 +26283,7 @@
         <v>326</v>
       </c>
       <c r="B326">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -26435,7 +26435,7 @@
         <v>345</v>
       </c>
       <c r="B345">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -26451,7 +26451,7 @@
         <v>347</v>
       </c>
       <c r="B347">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -26499,7 +26499,7 @@
         <v>353</v>
       </c>
       <c r="B353">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -26547,7 +26547,7 @@
         <v>359</v>
       </c>
       <c r="B359">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -26563,7 +26563,7 @@
         <v>361</v>
       </c>
       <c r="B361">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -26723,7 +26723,7 @@
         <v>381</v>
       </c>
       <c r="B381">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -26779,7 +26779,7 @@
         <v>388</v>
       </c>
       <c r="B388">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389" spans="1:2">
@@ -26851,7 +26851,7 @@
         <v>397</v>
       </c>
       <c r="B397">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="398" spans="1:2">
@@ -27091,7 +27091,7 @@
         <v>427</v>
       </c>
       <c r="B427">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="428" spans="1:2">
@@ -27411,7 +27411,7 @@
         <v>467</v>
       </c>
       <c r="B467">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="468" spans="1:2">
@@ -27643,7 +27643,7 @@
         <v>496</v>
       </c>
       <c r="B496">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="497" spans="1:2">
@@ -27715,7 +27715,7 @@
         <v>505</v>
       </c>
       <c r="B505">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="506" spans="1:2">
@@ -27763,7 +27763,7 @@
         <v>511</v>
       </c>
       <c r="B511">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="512" spans="1:2">
@@ -28075,7 +28075,7 @@
         <v>550</v>
       </c>
       <c r="B550">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="551" spans="1:2">
@@ -28083,7 +28083,7 @@
         <v>551</v>
       </c>
       <c r="B551">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="552" spans="1:2">
@@ -28187,7 +28187,7 @@
         <v>564</v>
       </c>
       <c r="B564">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="565" spans="1:2">
@@ -28275,7 +28275,7 @@
         <v>575</v>
       </c>
       <c r="B575">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="576" spans="1:2">
@@ -28443,7 +28443,7 @@
         <v>596</v>
       </c>
       <c r="B596">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="597" spans="1:2">
@@ -28635,7 +28635,7 @@
         <v>620</v>
       </c>
       <c r="B620">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="621" spans="1:2">
@@ -28811,7 +28811,7 @@
         <v>642</v>
       </c>
       <c r="B642">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="643" spans="1:2">
@@ -28835,7 +28835,7 @@
         <v>645</v>
       </c>
       <c r="B645">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="646" spans="1:2">
@@ -28883,7 +28883,7 @@
         <v>651</v>
       </c>
       <c r="B651">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="652" spans="1:2">
@@ -29019,7 +29019,7 @@
         <v>668</v>
       </c>
       <c r="B668">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="669" spans="1:2">
@@ -29027,7 +29027,7 @@
         <v>669</v>
       </c>
       <c r="B669">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="670" spans="1:2">
@@ -29483,7 +29483,7 @@
         <v>726</v>
       </c>
       <c r="B726">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="727" spans="1:2">
@@ -29635,7 +29635,7 @@
         <v>745</v>
       </c>
       <c r="B745">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="746" spans="1:2">
@@ -29907,7 +29907,7 @@
         <v>779</v>
       </c>
       <c r="B779">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="780" spans="1:2">
@@ -29987,7 +29987,7 @@
         <v>789</v>
       </c>
       <c r="B789">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="790" spans="1:2">
@@ -30003,7 +30003,7 @@
         <v>791</v>
       </c>
       <c r="B791">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="792" spans="1:2">
@@ -30059,7 +30059,7 @@
         <v>798</v>
       </c>
       <c r="B798">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="799" spans="1:2">
@@ -30203,7 +30203,7 @@
         <v>816</v>
       </c>
       <c r="B816">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="817" spans="1:2">
@@ -30891,7 +30891,7 @@
         <v>902</v>
       </c>
       <c r="B902">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="903" spans="1:2">
@@ -30987,7 +30987,7 @@
         <v>914</v>
       </c>
       <c r="B914">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="915" spans="1:2">
@@ -31147,7 +31147,7 @@
         <v>934</v>
       </c>
       <c r="B934">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="935" spans="1:2">
@@ -31171,7 +31171,7 @@
         <v>937</v>
       </c>
       <c r="B937">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="938" spans="1:2">
@@ -31323,7 +31323,7 @@
         <v>956</v>
       </c>
       <c r="B956">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="957" spans="1:2">
@@ -31379,7 +31379,7 @@
         <v>963</v>
       </c>
       <c r="B963">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="964" spans="1:2">
@@ -31531,7 +31531,7 @@
         <v>982</v>
       </c>
       <c r="B982">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="983" spans="1:2">
@@ -31563,7 +31563,7 @@
         <v>986</v>
       </c>
       <c r="B986">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="987" spans="1:2">
@@ -31579,7 +31579,7 @@
         <v>988</v>
       </c>
       <c r="B988">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="989" spans="1:2">
@@ -31627,7 +31627,7 @@
         <v>994</v>
       </c>
       <c r="B994">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="995" spans="1:2">
@@ -31747,7 +31747,7 @@
         <v>1009</v>
       </c>
       <c r="B1009">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1010" spans="1:2">
@@ -31883,7 +31883,7 @@
         <v>1026</v>
       </c>
       <c r="B1026">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1027" spans="1:2">
@@ -31979,7 +31979,7 @@
         <v>1038</v>
       </c>
       <c r="B1038">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1039" spans="1:2">
@@ -32003,7 +32003,7 @@
         <v>1041</v>
       </c>
       <c r="B1041">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1042" spans="1:2">
@@ -32307,7 +32307,7 @@
         <v>1079</v>
       </c>
       <c r="B1079">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1080" spans="1:2">
@@ -32403,7 +32403,7 @@
         <v>1091</v>
       </c>
       <c r="B1091">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1092" spans="1:2">
@@ -32451,7 +32451,7 @@
         <v>1097</v>
       </c>
       <c r="B1097">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1098" spans="1:2">
@@ -32579,7 +32579,7 @@
         <v>1113</v>
       </c>
       <c r="B1113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1114" spans="1:2">
@@ -32683,7 +32683,7 @@
         <v>1126</v>
       </c>
       <c r="B1126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1127" spans="1:2">
@@ -32851,7 +32851,7 @@
         <v>1147</v>
       </c>
       <c r="B1147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1148" spans="1:2">
@@ -32947,7 +32947,7 @@
         <v>1159</v>
       </c>
       <c r="B1159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1160" spans="1:2">
@@ -33139,7 +33139,7 @@
         <v>1183</v>
       </c>
       <c r="B1183">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1184" spans="1:2">
@@ -33203,7 +33203,7 @@
         <v>1191</v>
       </c>
       <c r="B1191">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1192" spans="1:2">
@@ -33555,7 +33555,7 @@
         <v>1235</v>
       </c>
       <c r="B1235">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1236" spans="1:2">
@@ -33595,7 +33595,7 @@
         <v>1240</v>
       </c>
       <c r="B1240">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1241" spans="1:2">
@@ -33787,7 +33787,7 @@
         <v>1264</v>
       </c>
       <c r="B1264">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1265" spans="1:2">
@@ -33875,7 +33875,7 @@
         <v>1275</v>
       </c>
       <c r="B1275">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1276" spans="1:2">
@@ -33955,7 +33955,7 @@
         <v>1285</v>
       </c>
       <c r="B1285">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1286" spans="1:2">
@@ -34467,7 +34467,7 @@
         <v>1349</v>
       </c>
       <c r="B1349">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1350" spans="1:2">
@@ -34683,7 +34683,7 @@
         <v>1376</v>
       </c>
       <c r="B1376">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1377" spans="1:2">
@@ -34963,7 +34963,7 @@
         <v>1411</v>
       </c>
       <c r="B1411">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1412" spans="1:2">
@@ -35131,7 +35131,7 @@
         <v>1432</v>
       </c>
       <c r="B1432">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1433" spans="1:2">
@@ -35315,7 +35315,7 @@
         <v>1455</v>
       </c>
       <c r="B1455">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1456" spans="1:2">
@@ -35699,7 +35699,7 @@
         <v>1503</v>
       </c>
       <c r="B1503">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1504" spans="1:2">
@@ -35779,7 +35779,7 @@
         <v>1513</v>
       </c>
       <c r="B1513">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1514" spans="1:2">
@@ -35819,7 +35819,7 @@
         <v>1518</v>
       </c>
       <c r="B1518">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1519" spans="1:2">
@@ -36019,7 +36019,7 @@
         <v>1543</v>
       </c>
       <c r="B1543">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1544" spans="1:2">
@@ -36131,7 +36131,7 @@
         <v>1557</v>
       </c>
       <c r="B1557">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1558" spans="1:2">
@@ -36139,7 +36139,7 @@
         <v>1558</v>
       </c>
       <c r="B1558">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1559" spans="1:2">
@@ -36267,7 +36267,7 @@
         <v>1574</v>
       </c>
       <c r="B1574">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1575" spans="1:2">
@@ -36515,7 +36515,7 @@
         <v>1605</v>
       </c>
       <c r="B1605">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1606" spans="1:2">
@@ -36683,7 +36683,7 @@
         <v>1626</v>
       </c>
       <c r="B1626">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1627" spans="1:2">
@@ -36691,7 +36691,7 @@
         <v>1627</v>
       </c>
       <c r="B1627">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1628" spans="1:2">
@@ -36803,7 +36803,7 @@
         <v>1641</v>
       </c>
       <c r="B1641">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1642" spans="1:2">
@@ -36819,7 +36819,7 @@
         <v>1643</v>
       </c>
       <c r="B1643">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1644" spans="1:2">
@@ -36843,7 +36843,7 @@
         <v>1646</v>
       </c>
       <c r="B1646">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1647" spans="1:2">
@@ -36899,7 +36899,7 @@
         <v>1653</v>
       </c>
       <c r="B1653">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1654" spans="1:2">
@@ -36947,7 +36947,7 @@
         <v>1659</v>
       </c>
       <c r="B1659">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1660" spans="1:2">
@@ -37027,7 +37027,7 @@
         <v>1669</v>
       </c>
       <c r="B1669">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1670" spans="1:2">
@@ -37395,7 +37395,7 @@
         <v>1715</v>
       </c>
       <c r="B1715">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1716" spans="1:2">
@@ -37595,7 +37595,7 @@
         <v>1740</v>
       </c>
       <c r="B1740">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1741" spans="1:2">
@@ -37635,7 +37635,7 @@
         <v>1745</v>
       </c>
       <c r="B1745">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1746" spans="1:2">
@@ -37643,7 +37643,7 @@
         <v>1746</v>
       </c>
       <c r="B1746">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1747" spans="1:2">
@@ -37691,7 +37691,7 @@
         <v>1752</v>
       </c>
       <c r="B1752">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1753" spans="1:2">
@@ -37763,7 +37763,7 @@
         <v>1761</v>
       </c>
       <c r="B1761">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1762" spans="1:2">
@@ -37875,7 +37875,7 @@
         <v>1775</v>
       </c>
       <c r="B1775">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1776" spans="1:2">
@@ -38131,7 +38131,7 @@
         <v>1807</v>
       </c>
       <c r="B1807">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1808" spans="1:2">
@@ -38635,7 +38635,7 @@
         <v>1870</v>
       </c>
       <c r="B1870">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1871" spans="1:2">
@@ -38675,7 +38675,7 @@
         <v>1875</v>
       </c>
       <c r="B1875">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1876" spans="1:2">
@@ -38699,7 +38699,7 @@
         <v>1878</v>
       </c>
       <c r="B1878">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1879" spans="1:2">
@@ -38723,7 +38723,7 @@
         <v>1881</v>
       </c>
       <c r="B1881">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1882" spans="1:2">
@@ -38795,7 +38795,7 @@
         <v>1890</v>
       </c>
       <c r="B1890">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1891" spans="1:2">
@@ -38835,7 +38835,7 @@
         <v>1895</v>
       </c>
       <c r="B1895">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1896" spans="1:2">
@@ -39091,7 +39091,7 @@
         <v>1927</v>
       </c>
       <c r="B1927">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1928" spans="1:2">
@@ -39131,7 +39131,7 @@
         <v>1932</v>
       </c>
       <c r="B1932">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1933" spans="1:2">
@@ -39155,7 +39155,7 @@
         <v>1935</v>
       </c>
       <c r="B1935">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1936" spans="1:2">
@@ -39171,7 +39171,7 @@
         <v>1937</v>
       </c>
       <c r="B1937">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1938" spans="1:2">
@@ -39211,7 +39211,7 @@
         <v>1942</v>
       </c>
       <c r="B1942">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1943" spans="1:2">
@@ -39387,7 +39387,7 @@
         <v>1964</v>
       </c>
       <c r="B1964">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1965" spans="1:2">
@@ -39435,7 +39435,7 @@
         <v>1970</v>
       </c>
       <c r="B1970">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1971" spans="1:2">
@@ -39475,7 +39475,7 @@
         <v>1975</v>
       </c>
       <c r="B1975">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1976" spans="1:2">
@@ -39523,7 +39523,7 @@
         <v>1981</v>
       </c>
       <c r="B1981">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1982" spans="1:2">
@@ -39651,7 +39651,7 @@
         <v>1997</v>
       </c>
       <c r="B1997">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1998" spans="1:2">
@@ -39747,7 +39747,7 @@
         <v>2009</v>
       </c>
       <c r="B2009">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2010" spans="1:2">
@@ -40035,7 +40035,7 @@
         <v>2045</v>
       </c>
       <c r="B2045">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2046" spans="1:2">
@@ -40179,7 +40179,7 @@
         <v>2063</v>
       </c>
       <c r="B2063">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2064" spans="1:2">
@@ -40347,7 +40347,7 @@
         <v>2084</v>
       </c>
       <c r="B2084">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2085" spans="1:2">
@@ -40395,7 +40395,7 @@
         <v>2090</v>
       </c>
       <c r="B2090">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2091" spans="1:2">
@@ -40451,7 +40451,7 @@
         <v>2097</v>
       </c>
       <c r="B2097">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2098" spans="1:2">
@@ -40467,7 +40467,7 @@
         <v>2099</v>
       </c>
       <c r="B2099">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2100" spans="1:2">
@@ -40539,7 +40539,7 @@
         <v>2108</v>
       </c>
       <c r="B2108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2109" spans="1:2">
@@ -40563,7 +40563,7 @@
         <v>2111</v>
       </c>
       <c r="B2111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2112" spans="1:2">
@@ -40571,7 +40571,7 @@
         <v>2112</v>
       </c>
       <c r="B2112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2113" spans="1:2">
@@ -40651,7 +40651,7 @@
         <v>2122</v>
       </c>
       <c r="B2122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2123" spans="1:2">
@@ -40715,7 +40715,7 @@
         <v>2130</v>
       </c>
       <c r="B2130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2131" spans="1:2">
@@ -40955,7 +40955,7 @@
         <v>2160</v>
       </c>
       <c r="B2160">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2161" spans="1:2">
@@ -41307,7 +41307,7 @@
         <v>2204</v>
       </c>
       <c r="B2204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2205" spans="1:2">
@@ -41363,7 +41363,7 @@
         <v>2211</v>
       </c>
       <c r="B2211">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2212" spans="1:2">
@@ -41539,7 +41539,7 @@
         <v>2233</v>
       </c>
       <c r="B2233">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2234" spans="1:2">
@@ -41643,7 +41643,7 @@
         <v>2246</v>
       </c>
       <c r="B2246">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2247" spans="1:2">
@@ -41659,7 +41659,7 @@
         <v>2248</v>
       </c>
       <c r="B2248">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2249" spans="1:2">
@@ -41675,7 +41675,7 @@
         <v>2250</v>
       </c>
       <c r="B2250">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2251" spans="1:2">
@@ -41715,7 +41715,7 @@
         <v>2255</v>
       </c>
       <c r="B2255">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2256" spans="1:2">
@@ -41771,7 +41771,7 @@
         <v>2262</v>
       </c>
       <c r="B2262">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2263" spans="1:2">
@@ -41835,7 +41835,7 @@
         <v>2270</v>
       </c>
       <c r="B2270">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2271" spans="1:2">
@@ -41939,7 +41939,7 @@
         <v>2283</v>
       </c>
       <c r="B2283">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2284" spans="1:2">
@@ -41979,7 +41979,7 @@
         <v>2288</v>
       </c>
       <c r="B2288">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2289" spans="1:2">
@@ -41995,7 +41995,7 @@
         <v>2290</v>
       </c>
       <c r="B2290">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2291" spans="1:2">
@@ -42027,7 +42027,7 @@
         <v>2294</v>
       </c>
       <c r="B2294">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2295" spans="1:2">
@@ -42155,7 +42155,7 @@
         <v>2310</v>
       </c>
       <c r="B2310">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2311" spans="1:2">
@@ -42307,7 +42307,7 @@
         <v>2329</v>
       </c>
       <c r="B2329">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2330" spans="1:2">
@@ -42315,7 +42315,7 @@
         <v>2330</v>
       </c>
       <c r="B2330">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2331" spans="1:2">
@@ -42435,7 +42435,7 @@
         <v>2345</v>
       </c>
       <c r="B2345">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2346" spans="1:2">
@@ -42707,7 +42707,7 @@
         <v>2379</v>
       </c>
       <c r="B2379">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2380" spans="1:2">
@@ -42795,7 +42795,7 @@
         <v>2390</v>
       </c>
       <c r="B2390">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2391" spans="1:2">
@@ -42867,7 +42867,7 @@
         <v>2399</v>
       </c>
       <c r="B2399">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2400" spans="1:2">
@@ -43155,7 +43155,7 @@
         <v>2435</v>
       </c>
       <c r="B2435">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2436" spans="1:2">
@@ -43339,7 +43339,7 @@
         <v>2458</v>
       </c>
       <c r="B2458">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2459" spans="1:2">
@@ -43587,7 +43587,7 @@
         <v>2489</v>
       </c>
       <c r="B2489">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2490" spans="1:2">
@@ -43731,7 +43731,7 @@
         <v>2507</v>
       </c>
       <c r="B2507">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2508" spans="1:2">
@@ -43931,7 +43931,7 @@
         <v>2532</v>
       </c>
       <c r="B2532">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2533" spans="1:2">
@@ -44243,7 +44243,7 @@
         <v>2571</v>
       </c>
       <c r="B2571">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2572" spans="1:2">
@@ -44275,7 +44275,7 @@
         <v>2575</v>
       </c>
       <c r="B2575">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2576" spans="1:2">
@@ -44491,7 +44491,7 @@
         <v>2602</v>
       </c>
       <c r="B2602">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2603" spans="1:2">
@@ -44507,7 +44507,7 @@
         <v>2604</v>
       </c>
       <c r="B2604">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2605" spans="1:2">
@@ -44547,7 +44547,7 @@
         <v>2609</v>
       </c>
       <c r="B2609">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2610" spans="1:2">
@@ -44699,7 +44699,7 @@
         <v>2628</v>
       </c>
       <c r="B2628">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2629" spans="1:2">
@@ -44763,7 +44763,7 @@
         <v>2636</v>
       </c>
       <c r="B2636">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2637" spans="1:2">
@@ -44787,7 +44787,7 @@
         <v>2639</v>
       </c>
       <c r="B2639">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2640" spans="1:2">
@@ -44867,7 +44867,7 @@
         <v>2649</v>
       </c>
       <c r="B2649">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2650" spans="1:2">
@@ -45003,7 +45003,7 @@
         <v>2666</v>
       </c>
       <c r="B2666">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2667" spans="1:2">
@@ -45155,7 +45155,7 @@
         <v>2685</v>
       </c>
       <c r="B2685">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2686" spans="1:2">
@@ -45283,7 +45283,7 @@
         <v>2701</v>
       </c>
       <c r="B2701">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2702" spans="1:2">
@@ -45531,7 +45531,7 @@
         <v>2732</v>
       </c>
       <c r="B2732">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2733" spans="1:2">
@@ -45579,7 +45579,7 @@
         <v>2738</v>
       </c>
       <c r="B2738">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2739" spans="1:2">
@@ -45627,7 +45627,7 @@
         <v>2744</v>
       </c>
       <c r="B2744">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2745" spans="1:2">
@@ -45907,7 +45907,7 @@
         <v>2779</v>
       </c>
       <c r="B2779">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2780" spans="1:2">
@@ -45995,7 +45995,7 @@
         <v>2790</v>
       </c>
       <c r="B2790">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2791" spans="1:2">
@@ -46227,7 +46227,7 @@
         <v>2819</v>
       </c>
       <c r="B2819">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2820" spans="1:2">
@@ -46331,7 +46331,7 @@
         <v>2832</v>
       </c>
       <c r="B2832">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2833" spans="1:2">
@@ -46347,7 +46347,7 @@
         <v>2834</v>
       </c>
       <c r="B2834">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2835" spans="1:2">
@@ -46539,7 +46539,7 @@
         <v>2858</v>
       </c>
       <c r="B2858">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2859" spans="1:2">
@@ -46627,7 +46627,7 @@
         <v>2869</v>
       </c>
       <c r="B2869">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2870" spans="1:2">
@@ -46683,7 +46683,7 @@
         <v>2876</v>
       </c>
       <c r="B2876">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2877" spans="1:2">
@@ -47011,7 +47011,7 @@
         <v>2917</v>
       </c>
       <c r="B2917">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2918" spans="1:2">
@@ -47019,7 +47019,7 @@
         <v>2918</v>
       </c>
       <c r="B2918">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2919" spans="1:2">
@@ -47163,7 +47163,7 @@
         <v>2936</v>
       </c>
       <c r="B2936">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2937" spans="1:2">
@@ -47275,7 +47275,7 @@
         <v>2950</v>
       </c>
       <c r="B2950">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2951" spans="1:2">
@@ -47291,7 +47291,7 @@
         <v>2952</v>
       </c>
       <c r="B2952">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2953" spans="1:2">
@@ -47483,7 +47483,7 @@
         <v>2976</v>
       </c>
       <c r="B2976">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2977" spans="1:2">
@@ -47531,7 +47531,7 @@
         <v>2982</v>
       </c>
       <c r="B2982">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2983" spans="1:2">
@@ -47571,7 +47571,7 @@
         <v>2987</v>
       </c>
       <c r="B2987">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2988" spans="1:2">
@@ -48083,7 +48083,7 @@
         <v>3051</v>
       </c>
       <c r="B3051">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3052" spans="1:2">
@@ -48147,7 +48147,7 @@
         <v>3059</v>
       </c>
       <c r="B3059">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3060" spans="1:2">
@@ -48203,7 +48203,7 @@
         <v>3066</v>
       </c>
       <c r="B3066">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3067" spans="1:2">
@@ -48211,7 +48211,7 @@
         <v>3067</v>
       </c>
       <c r="B3067">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3068" spans="1:2">
@@ -48379,7 +48379,7 @@
         <v>3088</v>
       </c>
       <c r="B3088">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3089" spans="1:2">
@@ -48395,7 +48395,7 @@
         <v>3090</v>
       </c>
       <c r="B3090">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3091" spans="1:2">
@@ -48771,7 +48771,7 @@
         <v>3137</v>
       </c>
       <c r="B3137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3138" spans="1:2">
@@ -48987,7 +48987,7 @@
         <v>3164</v>
       </c>
       <c r="B3164">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3165" spans="1:2">
@@ -49043,7 +49043,7 @@
         <v>3171</v>
       </c>
       <c r="B3171">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3172" spans="1:2">
@@ -49275,7 +49275,7 @@
         <v>3200</v>
       </c>
       <c r="B3200">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3201" spans="1:2">
@@ -49563,7 +49563,7 @@
         <v>3236</v>
       </c>
       <c r="B3236">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3237" spans="1:2">
@@ -49835,7 +49835,7 @@
         <v>3270</v>
       </c>
       <c r="B3270">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3271" spans="1:2">
@@ -50019,7 +50019,7 @@
         <v>3293</v>
       </c>
       <c r="B3293">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3294" spans="1:2">
@@ -50059,7 +50059,7 @@
         <v>3298</v>
       </c>
       <c r="B3298">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3299" spans="1:2">
@@ -50203,7 +50203,7 @@
         <v>3316</v>
       </c>
       <c r="B3316">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3317" spans="1:2">
@@ -50339,7 +50339,7 @@
         <v>3333</v>
       </c>
       <c r="B3333">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3334" spans="1:2">
@@ -50611,7 +50611,7 @@
         <v>3367</v>
       </c>
       <c r="B3367">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3368" spans="1:2">
@@ -50771,7 +50771,7 @@
         <v>3387</v>
       </c>
       <c r="B3387">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3388" spans="1:2">
@@ -51035,7 +51035,7 @@
         <v>3420</v>
       </c>
       <c r="B3420">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3421" spans="1:2">
@@ -51243,7 +51243,7 @@
         <v>3446</v>
       </c>
       <c r="B3446">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3447" spans="1:2">
@@ -51579,7 +51579,7 @@
         <v>3488</v>
       </c>
       <c r="B3488">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3489" spans="1:2">
@@ -51707,7 +51707,7 @@
         <v>3504</v>
       </c>
       <c r="B3504">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3505" spans="1:2">
@@ -51739,7 +51739,7 @@
         <v>3508</v>
       </c>
       <c r="B3508">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3509" spans="1:2">
@@ -51955,7 +51955,7 @@
         <v>3535</v>
       </c>
       <c r="B3535">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3536" spans="1:2">
@@ -52107,7 +52107,7 @@
         <v>3554</v>
       </c>
       <c r="B3554">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3555" spans="1:2">
@@ -52211,7 +52211,7 @@
         <v>3567</v>
       </c>
       <c r="B3567">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3568" spans="1:2">
@@ -52467,7 +52467,7 @@
         <v>3599</v>
       </c>
       <c r="B3599">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3600" spans="1:2">
@@ -52499,7 +52499,7 @@
         <v>3603</v>
       </c>
       <c r="B3603">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3604" spans="1:2">
@@ -52515,7 +52515,7 @@
         <v>3605</v>
       </c>
       <c r="B3605">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3606" spans="1:2">
@@ -52611,7 +52611,7 @@
         <v>3617</v>
       </c>
       <c r="B3617">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3618" spans="1:2">
@@ -52907,7 +52907,7 @@
         <v>3654</v>
       </c>
       <c r="B3654">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3655" spans="1:2">
@@ -52963,7 +52963,7 @@
         <v>3661</v>
       </c>
       <c r="B3661">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3662" spans="1:2">
@@ -53003,7 +53003,7 @@
         <v>3666</v>
       </c>
       <c r="B3666">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3667" spans="1:2">
@@ -53243,7 +53243,7 @@
         <v>3696</v>
       </c>
       <c r="B3696">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3697" spans="1:2">
@@ -53299,7 +53299,7 @@
         <v>3703</v>
       </c>
       <c r="B3703">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3704" spans="1:2">
@@ -53331,7 +53331,7 @@
         <v>3707</v>
       </c>
       <c r="B3707">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3708" spans="1:2">
@@ -53427,7 +53427,7 @@
         <v>3719</v>
       </c>
       <c r="B3719">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3720" spans="1:2">
@@ -53459,7 +53459,7 @@
         <v>3723</v>
       </c>
       <c r="B3723">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3724" spans="1:2">
@@ -53499,7 +53499,7 @@
         <v>3728</v>
       </c>
       <c r="B3728">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3729" spans="1:2">
@@ -53819,7 +53819,7 @@
         <v>3768</v>
       </c>
       <c r="B3768">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3769" spans="1:2">
@@ -53947,7 +53947,7 @@
         <v>3784</v>
       </c>
       <c r="B3784">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3785" spans="1:2">
@@ -54043,7 +54043,7 @@
         <v>3796</v>
       </c>
       <c r="B3796">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3797" spans="1:2">
@@ -54243,7 +54243,7 @@
         <v>3821</v>
       </c>
       <c r="B3821">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3822" spans="1:2">
@@ -54307,7 +54307,7 @@
         <v>3829</v>
       </c>
       <c r="B3829">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3830" spans="1:2">
@@ -54491,7 +54491,7 @@
         <v>3852</v>
       </c>
       <c r="B3852">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3853" spans="1:2">
@@ -54699,7 +54699,7 @@
         <v>3878</v>
       </c>
       <c r="B3878">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3879" spans="1:2">
@@ -54819,7 +54819,7 @@
         <v>3893</v>
       </c>
       <c r="B3893">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3894" spans="1:2">
@@ -54875,7 +54875,7 @@
         <v>3900</v>
       </c>
       <c r="B3900">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3901" spans="1:2">
@@ -54907,7 +54907,7 @@
         <v>3904</v>
       </c>
       <c r="B3904">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3905" spans="1:2">
@@ -54963,7 +54963,7 @@
         <v>3911</v>
       </c>
       <c r="B3911">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3912" spans="1:2">
@@ -55099,7 +55099,7 @@
         <v>3928</v>
       </c>
       <c r="B3928">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3929" spans="1:2">
@@ -55147,7 +55147,7 @@
         <v>3934</v>
       </c>
       <c r="B3934">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3935" spans="1:2">
@@ -55187,7 +55187,7 @@
         <v>3939</v>
       </c>
       <c r="B3939">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3940" spans="1:2">
@@ -55323,7 +55323,7 @@
         <v>3956</v>
       </c>
       <c r="B3956">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3957" spans="1:2">
@@ -55347,7 +55347,7 @@
         <v>3959</v>
       </c>
       <c r="B3959">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3960" spans="1:2">
@@ -55419,7 +55419,7 @@
         <v>3968</v>
       </c>
       <c r="B3968">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3969" spans="1:2">
@@ -55483,7 +55483,7 @@
         <v>3976</v>
       </c>
       <c r="B3976">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3977" spans="1:2">
@@ -55539,7 +55539,7 @@
         <v>3983</v>
       </c>
       <c r="B3983">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3984" spans="1:2">
@@ -55563,7 +55563,7 @@
         <v>3986</v>
       </c>
       <c r="B3986">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3987" spans="1:2">
@@ -55691,7 +55691,7 @@
         <v>4002</v>
       </c>
       <c r="B4002">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4003" spans="1:2">
@@ -55803,7 +55803,7 @@
         <v>4016</v>
       </c>
       <c r="B4016">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4017" spans="1:2">
@@ -55923,7 +55923,7 @@
         <v>4031</v>
       </c>
       <c r="B4031">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4032" spans="1:2">
@@ -56299,7 +56299,7 @@
         <v>4078</v>
       </c>
       <c r="B4078">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4079" spans="1:2">
@@ -56403,7 +56403,7 @@
         <v>4091</v>
       </c>
       <c r="B4091">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4092" spans="1:2">
@@ -56763,7 +56763,7 @@
         <v>4136</v>
       </c>
       <c r="B4136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4137" spans="1:2">
@@ -56995,7 +56995,7 @@
         <v>4165</v>
       </c>
       <c r="B4165">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4166" spans="1:2">
@@ -57275,7 +57275,7 @@
         <v>4200</v>
       </c>
       <c r="B4200">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4201" spans="1:2">
@@ -57355,7 +57355,7 @@
         <v>4210</v>
       </c>
       <c r="B4210">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4211" spans="1:2">
@@ -57419,7 +57419,7 @@
         <v>4218</v>
       </c>
       <c r="B4218">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4219" spans="1:2">
@@ -57443,7 +57443,7 @@
         <v>4221</v>
       </c>
       <c r="B4221">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4222" spans="1:2">
@@ -57627,7 +57627,7 @@
         <v>4244</v>
       </c>
       <c r="B4244">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4245" spans="1:2">
@@ -57883,7 +57883,7 @@
         <v>4276</v>
       </c>
       <c r="B4276">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4277" spans="1:2">
@@ -58003,7 +58003,7 @@
         <v>4291</v>
       </c>
       <c r="B4291">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4292" spans="1:2">
@@ -58147,7 +58147,7 @@
         <v>4309</v>
       </c>
       <c r="B4309">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4310" spans="1:2">
@@ -58179,7 +58179,7 @@
         <v>4313</v>
       </c>
       <c r="B4313">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4314" spans="1:2">
@@ -58259,7 +58259,7 @@
         <v>4323</v>
       </c>
       <c r="B4323">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4324" spans="1:2">
@@ -58267,7 +58267,7 @@
         <v>4324</v>
       </c>
       <c r="B4324">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4325" spans="1:2">
@@ -58315,7 +58315,7 @@
         <v>4330</v>
       </c>
       <c r="B4330">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4331" spans="1:2">
@@ -58459,7 +58459,7 @@
         <v>4348</v>
       </c>
       <c r="B4348">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4349" spans="1:2">
@@ -58491,7 +58491,7 @@
         <v>4352</v>
       </c>
       <c r="B4352">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4353" spans="1:2">
@@ -58523,7 +58523,7 @@
         <v>4356</v>
       </c>
       <c r="B4356">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4357" spans="1:2">
@@ -58635,7 +58635,7 @@
         <v>4370</v>
       </c>
       <c r="B4370">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4371" spans="1:2">
@@ -58643,7 +58643,7 @@
         <v>4371</v>
       </c>
       <c r="B4371">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4372" spans="1:2">
@@ -58731,7 +58731,7 @@
         <v>4382</v>
       </c>
       <c r="B4382">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4383" spans="1:2">
@@ -58755,7 +58755,7 @@
         <v>4385</v>
       </c>
       <c r="B4385">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4386" spans="1:2">
@@ -59011,7 +59011,7 @@
         <v>4417</v>
       </c>
       <c r="B4417">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4418" spans="1:2">
@@ -59195,7 +59195,7 @@
         <v>4440</v>
       </c>
       <c r="B4440">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4441" spans="1:2">
@@ -59211,7 +59211,7 @@
         <v>4442</v>
       </c>
       <c r="B4442">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4443" spans="1:2">
@@ -59275,7 +59275,7 @@
         <v>4450</v>
       </c>
       <c r="B4450">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4451" spans="1:2">
@@ -59483,7 +59483,7 @@
         <v>4476</v>
       </c>
       <c r="B4476">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4477" spans="1:2">
@@ -59579,7 +59579,7 @@
         <v>4488</v>
       </c>
       <c r="B4488">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4489" spans="1:2">
@@ -59827,7 +59827,7 @@
         <v>4519</v>
       </c>
       <c r="B4519">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4520" spans="1:2">
@@ -59939,7 +59939,7 @@
         <v>4533</v>
       </c>
       <c r="B4533">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4534" spans="1:2">
@@ -60075,7 +60075,7 @@
         <v>4550</v>
       </c>
       <c r="B4550">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4551" spans="1:2">
@@ -60107,7 +60107,7 @@
         <v>4554</v>
       </c>
       <c r="B4554">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4555" spans="1:2">
@@ -60155,7 +60155,7 @@
         <v>4560</v>
       </c>
       <c r="B4560">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4561" spans="1:2">
@@ -60299,7 +60299,7 @@
         <v>4578</v>
       </c>
       <c r="B4578">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4579" spans="1:2">
@@ -60347,7 +60347,7 @@
         <v>4584</v>
       </c>
       <c r="B4584">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4585" spans="1:2">
@@ -60699,7 +60699,7 @@
         <v>4628</v>
       </c>
       <c r="B4628">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4629" spans="1:2">
@@ -60723,7 +60723,7 @@
         <v>4631</v>
       </c>
       <c r="B4631">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4632" spans="1:2">
@@ -60771,7 +60771,7 @@
         <v>4637</v>
       </c>
       <c r="B4637">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4638" spans="1:2">
@@ -60787,7 +60787,7 @@
         <v>4639</v>
       </c>
       <c r="B4639">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4640" spans="1:2">
@@ -60827,7 +60827,7 @@
         <v>4644</v>
       </c>
       <c r="B4644">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4645" spans="1:2">
@@ -61003,7 +61003,7 @@
         <v>4666</v>
       </c>
       <c r="B4666">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4667" spans="1:2">
@@ -61451,7 +61451,7 @@
         <v>4722</v>
       </c>
       <c r="B4722">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4723" spans="1:2">
@@ -61563,7 +61563,7 @@
         <v>4736</v>
       </c>
       <c r="B4736">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4737" spans="1:2">
@@ -61643,7 +61643,7 @@
         <v>4746</v>
       </c>
       <c r="B4746">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4747" spans="1:2">
@@ -61675,7 +61675,7 @@
         <v>4750</v>
       </c>
       <c r="B4750">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4751" spans="1:2">
@@ -61691,7 +61691,7 @@
         <v>4752</v>
       </c>
       <c r="B4752">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4753" spans="1:2">
@@ -61867,7 +61867,7 @@
         <v>4774</v>
       </c>
       <c r="B4774">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4775" spans="1:2">
@@ -62395,7 +62395,7 @@
         <v>4840</v>
       </c>
       <c r="B4840">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4841" spans="1:2">
@@ -62523,7 +62523,7 @@
         <v>4856</v>
       </c>
       <c r="B4856">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4857" spans="1:2">
@@ -62755,7 +62755,7 @@
         <v>4885</v>
       </c>
       <c r="B4885">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4886" spans="1:2">
@@ -62955,7 +62955,7 @@
         <v>4910</v>
       </c>
       <c r="B4910">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4911" spans="1:2">
@@ -63275,7 +63275,7 @@
         <v>4950</v>
       </c>
       <c r="B4950">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4951" spans="1:2">
@@ -63291,7 +63291,7 @@
         <v>4952</v>
       </c>
       <c r="B4952">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4953" spans="1:2">
@@ -63675,7 +63675,7 @@
         <v>5000</v>
       </c>
       <c r="B5000">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5001" spans="1:2">
@@ -63739,7 +63739,7 @@
         <v>5008</v>
       </c>
       <c r="B5008">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5009" spans="1:2">
@@ -63923,7 +63923,7 @@
         <v>5031</v>
       </c>
       <c r="B5031">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5032" spans="1:2">
@@ -63939,7 +63939,7 @@
         <v>5033</v>
       </c>
       <c r="B5033">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5034" spans="1:2">
@@ -64155,7 +64155,7 @@
         <v>5060</v>
       </c>
       <c r="B5060">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5061" spans="1:2">
@@ -64267,7 +64267,7 @@
         <v>5074</v>
       </c>
       <c r="B5074">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5075" spans="1:2">
@@ -64315,7 +64315,7 @@
         <v>5080</v>
       </c>
       <c r="B5080">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5081" spans="1:2">
@@ -64515,7 +64515,7 @@
         <v>5105</v>
       </c>
       <c r="B5105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5106" spans="1:2">
@@ -64947,7 +64947,7 @@
         <v>5159</v>
       </c>
       <c r="B5159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5160" spans="1:2">
@@ -65107,7 +65107,7 @@
         <v>5179</v>
       </c>
       <c r="B5179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5180" spans="1:2">
@@ -65267,7 +65267,7 @@
         <v>5199</v>
       </c>
       <c r="B5199">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5200" spans="1:2">
@@ -65395,7 +65395,7 @@
         <v>5215</v>
       </c>
       <c r="B5215">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5216" spans="1:2">
@@ -65475,7 +65475,7 @@
         <v>5225</v>
       </c>
       <c r="B5225">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5226" spans="1:2">
@@ -65523,7 +65523,7 @@
         <v>5231</v>
       </c>
       <c r="B5231">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5232" spans="1:2">
@@ -65691,7 +65691,7 @@
         <v>5252</v>
       </c>
       <c r="B5252">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5253" spans="1:2">
@@ -65771,7 +65771,7 @@
         <v>5262</v>
       </c>
       <c r="B5262">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5263" spans="1:2">
@@ -65835,7 +65835,7 @@
         <v>5270</v>
       </c>
       <c r="B5270">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5271" spans="1:2">
@@ -65875,7 +65875,7 @@
         <v>5275</v>
       </c>
       <c r="B5275">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5276" spans="1:2">
@@ -66019,7 +66019,7 @@
         <v>5293</v>
       </c>
       <c r="B5293">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5294" spans="1:2">
@@ -66371,7 +66371,7 @@
         <v>5337</v>
       </c>
       <c r="B5337">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5338" spans="1:2">
@@ -66691,7 +66691,7 @@
         <v>5377</v>
       </c>
       <c r="B5377">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5378" spans="1:2">
@@ -66931,7 +66931,7 @@
         <v>5407</v>
       </c>
       <c r="B5407">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5408" spans="1:2">
@@ -66955,7 +66955,7 @@
         <v>5410</v>
       </c>
       <c r="B5410">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5411" spans="1:2">
@@ -67227,7 +67227,7 @@
         <v>5444</v>
       </c>
       <c r="B5444">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5445" spans="1:2">
@@ -67275,7 +67275,7 @@
         <v>5450</v>
       </c>
       <c r="B5450">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5451" spans="1:2">
@@ -67547,7 +67547,7 @@
         <v>5484</v>
       </c>
       <c r="B5484">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5485" spans="1:2">
@@ -67595,7 +67595,7 @@
         <v>5490</v>
       </c>
       <c r="B5490">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5491" spans="1:2">
@@ -67603,7 +67603,7 @@
         <v>5491</v>
       </c>
       <c r="B5491">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5492" spans="1:2">
@@ -67875,7 +67875,7 @@
         <v>5525</v>
       </c>
       <c r="B5525">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5526" spans="1:2">
@@ -68027,7 +68027,7 @@
         <v>5544</v>
       </c>
       <c r="B5544">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5545" spans="1:2">
@@ -68035,7 +68035,7 @@
         <v>5545</v>
       </c>
       <c r="B5545">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5546" spans="1:2">
@@ -68075,7 +68075,7 @@
         <v>5550</v>
       </c>
       <c r="B5550">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5551" spans="1:2">
@@ -68147,7 +68147,7 @@
         <v>5559</v>
       </c>
       <c r="B5559">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5560" spans="1:2">
@@ -68155,7 +68155,7 @@
         <v>5560</v>
       </c>
       <c r="B5560">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5561" spans="1:2">
@@ -68363,7 +68363,7 @@
         <v>5586</v>
       </c>
       <c r="B5586">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5587" spans="1:2">
@@ -68827,7 +68827,7 @@
         <v>5644</v>
       </c>
       <c r="B5644">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5645" spans="1:2">
@@ -68963,7 +68963,7 @@
         <v>5661</v>
       </c>
       <c r="B5661">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5662" spans="1:2">
@@ -69059,7 +69059,7 @@
         <v>5673</v>
       </c>
       <c r="B5673">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5674" spans="1:2">
@@ -69083,7 +69083,7 @@
         <v>5676</v>
       </c>
       <c r="B5676">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5677" spans="1:2">
@@ -69107,7 +69107,7 @@
         <v>5679</v>
       </c>
       <c r="B5679">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5680" spans="1:2">
@@ -69555,7 +69555,7 @@
         <v>5735</v>
       </c>
       <c r="B5735">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5736" spans="1:2">
@@ -70059,7 +70059,7 @@
         <v>5798</v>
       </c>
       <c r="B5798">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5799" spans="1:2">
@@ -70075,7 +70075,7 @@
         <v>5800</v>
       </c>
       <c r="B5800">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5801" spans="1:2">
@@ -70499,7 +70499,7 @@
         <v>5853</v>
       </c>
       <c r="B5853">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5854" spans="1:2">
@@ -70595,7 +70595,7 @@
         <v>5865</v>
       </c>
       <c r="B5865">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5866" spans="1:2">
@@ -70619,7 +70619,7 @@
         <v>5868</v>
       </c>
       <c r="B5868">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5869" spans="1:2">
@@ -70891,7 +70891,7 @@
         <v>5902</v>
       </c>
       <c r="B5902">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5903" spans="1:2">
@@ -71027,7 +71027,7 @@
         <v>5919</v>
       </c>
       <c r="B5919">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5920" spans="1:2">
@@ -71075,7 +71075,7 @@
         <v>5925</v>
       </c>
       <c r="B5925">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5926" spans="1:2">
@@ -71363,7 +71363,7 @@
         <v>5961</v>
       </c>
       <c r="B5961">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5962" spans="1:2">
@@ -71419,7 +71419,7 @@
         <v>5968</v>
       </c>
       <c r="B5968">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5969" spans="1:2">
@@ -71491,7 +71491,7 @@
         <v>5977</v>
       </c>
       <c r="B5977">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5978" spans="1:2">
@@ -71571,7 +71571,7 @@
         <v>5987</v>
       </c>
       <c r="B5987">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5988" spans="1:2">
@@ -72107,7 +72107,7 @@
         <v>6054</v>
       </c>
       <c r="B6054">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6055" spans="1:2">
@@ -72147,7 +72147,7 @@
         <v>6059</v>
       </c>
       <c r="B6059">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6060" spans="1:2">
@@ -72499,7 +72499,7 @@
         <v>6103</v>
       </c>
       <c r="B6103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6104" spans="1:2">
@@ -72507,7 +72507,7 @@
         <v>6104</v>
       </c>
       <c r="B6104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6105" spans="1:2">
@@ -72675,7 +72675,7 @@
         <v>6125</v>
       </c>
       <c r="B6125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6126" spans="1:2">
@@ -72971,7 +72971,7 @@
         <v>6162</v>
       </c>
       <c r="B6162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6163" spans="1:2">
@@ -73115,7 +73115,7 @@
         <v>6180</v>
       </c>
       <c r="B6180">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6181" spans="1:2">
@@ -73147,7 +73147,7 @@
         <v>6184</v>
       </c>
       <c r="B6184">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6185" spans="1:2">
@@ -73307,7 +73307,7 @@
         <v>6204</v>
       </c>
       <c r="B6204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6205" spans="1:2">
@@ -73427,7 +73427,7 @@
         <v>6219</v>
       </c>
       <c r="B6219">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6220" spans="1:2">
@@ -73475,7 +73475,7 @@
         <v>6225</v>
       </c>
       <c r="B6225">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6226" spans="1:2">
@@ -73907,7 +73907,7 @@
         <v>6279</v>
       </c>
       <c r="B6279">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6280" spans="1:2">
@@ -74187,7 +74187,7 @@
         <v>6314</v>
       </c>
       <c r="B6314">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6315" spans="1:2">
@@ -74251,7 +74251,7 @@
         <v>6322</v>
       </c>
       <c r="B6322">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6323" spans="1:2">
@@ -74323,7 +74323,7 @@
         <v>6331</v>
       </c>
       <c r="B6331">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6332" spans="1:2">
@@ -74803,7 +74803,7 @@
         <v>6391</v>
       </c>
       <c r="B6391">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6392" spans="1:2">
@@ -74891,7 +74891,7 @@
         <v>6402</v>
       </c>
       <c r="B6402">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6403" spans="1:2">
@@ -74931,7 +74931,7 @@
         <v>6407</v>
       </c>
       <c r="B6407">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6408" spans="1:2">
@@ -74987,7 +74987,7 @@
         <v>6414</v>
       </c>
       <c r="B6414">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6415" spans="1:2">
@@ -75163,7 +75163,7 @@
         <v>6436</v>
       </c>
       <c r="B6436">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6437" spans="1:2">
@@ -75619,7 +75619,7 @@
         <v>6493</v>
       </c>
       <c r="B6493">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6494" spans="1:2">
@@ -75779,7 +75779,7 @@
         <v>6513</v>
       </c>
       <c r="B6513">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6514" spans="1:2">
@@ -75811,7 +75811,7 @@
         <v>6517</v>
       </c>
       <c r="B6517">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6518" spans="1:2">
@@ -75851,7 +75851,7 @@
         <v>6522</v>
       </c>
       <c r="B6522">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6523" spans="1:2">
@@ -75923,7 +75923,7 @@
         <v>6531</v>
       </c>
       <c r="B6531">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6532" spans="1:2">
@@ -75939,7 +75939,7 @@
         <v>6533</v>
       </c>
       <c r="B6533">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6534" spans="1:2">
@@ -76019,7 +76019,7 @@
         <v>6543</v>
       </c>
       <c r="B6543">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6544" spans="1:2">
@@ -76219,7 +76219,7 @@
         <v>6568</v>
       </c>
       <c r="B6568">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6569" spans="1:2">
@@ -76227,7 +76227,7 @@
         <v>6569</v>
       </c>
       <c r="B6569">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6570" spans="1:2">
@@ -76451,7 +76451,7 @@
         <v>6597</v>
       </c>
       <c r="B6597">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6598" spans="1:2">
@@ -76643,7 +76643,7 @@
         <v>6621</v>
       </c>
       <c r="B6621">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6622" spans="1:2">
@@ -76787,7 +76787,7 @@
         <v>6639</v>
       </c>
       <c r="B6639">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6640" spans="1:2">
@@ -77099,7 +77099,7 @@
         <v>6678</v>
       </c>
       <c r="B6678">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6679" spans="1:2">
@@ -77219,7 +77219,7 @@
         <v>6693</v>
       </c>
       <c r="B6693">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6694" spans="1:2">
@@ -77299,7 +77299,7 @@
         <v>6703</v>
       </c>
       <c r="B6703">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6704" spans="1:2">
@@ -77331,7 +77331,7 @@
         <v>6707</v>
       </c>
       <c r="B6707">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6708" spans="1:2">
@@ -77347,7 +77347,7 @@
         <v>6709</v>
       </c>
       <c r="B6709">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6710" spans="1:2">
@@ -77379,7 +77379,7 @@
         <v>6713</v>
       </c>
       <c r="B6713">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6714" spans="1:2">
@@ -77459,7 +77459,7 @@
         <v>6723</v>
       </c>
       <c r="B6723">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6724" spans="1:2">
@@ -77723,7 +77723,7 @@
         <v>6756</v>
       </c>
       <c r="B6756">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6757" spans="1:2">
@@ -77819,7 +77819,7 @@
         <v>6768</v>
       </c>
       <c r="B6768">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6769" spans="1:2">
@@ -77899,7 +77899,7 @@
         <v>6778</v>
       </c>
       <c r="B6778">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6779" spans="1:2">
@@ -78083,7 +78083,7 @@
         <v>6801</v>
       </c>
       <c r="B6801">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6802" spans="1:2">
@@ -78147,7 +78147,7 @@
         <v>6809</v>
       </c>
       <c r="B6809">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6810" spans="1:2">
@@ -78155,7 +78155,7 @@
         <v>6810</v>
       </c>
       <c r="B6810">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6811" spans="1:2">
@@ -78163,7 +78163,7 @@
         <v>6811</v>
       </c>
       <c r="B6811">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6812" spans="1:2">
@@ -78667,7 +78667,7 @@
         <v>6874</v>
       </c>
       <c r="B6874">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6875" spans="1:2">
@@ -78739,7 +78739,7 @@
         <v>6883</v>
       </c>
       <c r="B6883">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6884" spans="1:2">
@@ -78763,7 +78763,7 @@
         <v>6886</v>
       </c>
       <c r="B6886">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6887" spans="1:2">
@@ -78851,7 +78851,7 @@
         <v>6897</v>
       </c>
       <c r="B6897">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6898" spans="1:2">
@@ -79035,7 +79035,7 @@
         <v>6920</v>
       </c>
       <c r="B6920">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6921" spans="1:2">
@@ -79659,7 +79659,7 @@
         <v>6998</v>
       </c>
       <c r="B6998">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6999" spans="1:2">
@@ -79707,7 +79707,7 @@
         <v>7004</v>
       </c>
       <c r="B7004">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7005" spans="1:2">
@@ -79939,7 +79939,7 @@
         <v>7033</v>
       </c>
       <c r="B7033">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7034" spans="1:2">
@@ -80179,7 +80179,7 @@
         <v>7063</v>
       </c>
       <c r="B7063">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7064" spans="1:2">
@@ -80219,7 +80219,7 @@
         <v>7068</v>
       </c>
       <c r="B7068">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7069" spans="1:2">
@@ -80235,7 +80235,7 @@
         <v>7070</v>
       </c>
       <c r="B7070">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7071" spans="1:2">
@@ -80267,7 +80267,7 @@
         <v>7074</v>
       </c>
       <c r="B7074">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7075" spans="1:2">
@@ -80347,7 +80347,7 @@
         <v>7084</v>
       </c>
       <c r="B7084">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7085" spans="1:2">
@@ -80395,7 +80395,7 @@
         <v>7090</v>
       </c>
       <c r="B7090">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7091" spans="1:2">
@@ -80435,7 +80435,7 @@
         <v>7095</v>
       </c>
       <c r="B7095">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7096" spans="1:2">
@@ -80939,7 +80939,7 @@
         <v>7158</v>
       </c>
       <c r="B7158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7159" spans="1:2">
@@ -81019,7 +81019,7 @@
         <v>7168</v>
       </c>
       <c r="B7168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7169" spans="1:2">
@@ -81075,7 +81075,7 @@
         <v>7175</v>
       </c>
       <c r="B7175">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7176" spans="1:2">
@@ -81107,7 +81107,7 @@
         <v>7179</v>
       </c>
       <c r="B7179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7180" spans="1:2">
@@ -81259,7 +81259,7 @@
         <v>7198</v>
       </c>
       <c r="B7198">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7199" spans="1:2">
@@ -81299,7 +81299,7 @@
         <v>7203</v>
       </c>
       <c r="B7203">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7204" spans="1:2">
@@ -81683,7 +81683,7 @@
         <v>7251</v>
       </c>
       <c r="B7251">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7252" spans="1:2">
@@ -82203,7 +82203,7 @@
         <v>7316</v>
       </c>
       <c r="B7316">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7317" spans="1:2">
@@ -82243,7 +82243,7 @@
         <v>7321</v>
       </c>
       <c r="B7321">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7322" spans="1:2">
@@ -82443,7 +82443,7 @@
         <v>7346</v>
       </c>
       <c r="B7346">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7347" spans="1:2">
@@ -82651,7 +82651,7 @@
         <v>7372</v>
       </c>
       <c r="B7372">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7373" spans="1:2">
@@ -82667,7 +82667,7 @@
         <v>7374</v>
       </c>
       <c r="B7374">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7375" spans="1:2">
@@ -82995,7 +82995,7 @@
         <v>7415</v>
       </c>
       <c r="B7415">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7416" spans="1:2">
@@ -83411,7 +83411,7 @@
         <v>7467</v>
       </c>
       <c r="B7467">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7468" spans="1:2">
@@ -83571,7 +83571,7 @@
         <v>7487</v>
       </c>
       <c r="B7487">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7488" spans="1:2">
@@ -83835,7 +83835,7 @@
         <v>7520</v>
       </c>
       <c r="B7520">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7521" spans="1:2">
@@ -83907,7 +83907,7 @@
         <v>7529</v>
       </c>
       <c r="B7529">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7530" spans="1:2">
@@ -84027,7 +84027,7 @@
         <v>7544</v>
       </c>
       <c r="B7544">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7545" spans="1:2">
@@ -84099,7 +84099,7 @@
         <v>7553</v>
       </c>
       <c r="B7553">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7554" spans="1:2">
@@ -84259,7 +84259,7 @@
         <v>7573</v>
       </c>
       <c r="B7573">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7574" spans="1:2">
@@ -84475,7 +84475,7 @@
         <v>7600</v>
       </c>
       <c r="B7600">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7601" spans="1:2">
@@ -84699,7 +84699,7 @@
         <v>7628</v>
       </c>
       <c r="B7628">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7629" spans="1:2">
@@ -84899,7 +84899,7 @@
         <v>7653</v>
       </c>
       <c r="B7653">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7654" spans="1:2">
@@ -84915,7 +84915,7 @@
         <v>7655</v>
       </c>
       <c r="B7655">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7656" spans="1:2">
@@ -85043,7 +85043,7 @@
         <v>7671</v>
       </c>
       <c r="B7671">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7672" spans="1:2">
@@ -85059,7 +85059,7 @@
         <v>7673</v>
       </c>
       <c r="B7673">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7674" spans="1:2">
@@ -85363,7 +85363,7 @@
         <v>7711</v>
       </c>
       <c r="B7711">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7712" spans="1:2">
@@ -85411,7 +85411,7 @@
         <v>7717</v>
       </c>
       <c r="B7717">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7718" spans="1:2">

</xml_diff>